<commit_message>
Fixed some minor bugs, upload the datas for the system
Last commit
</commit_message>
<xml_diff>
--- a/CS162-KTLT-Summer2020-Project Summary.xlsx
+++ b/CS162-KTLT-Summer2020-Project Summary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A52C59B-AD9B-460D-A8B1-DFBBB5C0F662}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C48F099-45C0-418C-8833-27A43350C4EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1345,14 +1345,14 @@
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Đầu đề 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Siêu kết nối" xfId="8" builtinId="8"/>
   </cellStyles>
   <dxfs count="18">
     <dxf>
@@ -2070,7 +2070,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -2164,11 +2164,10 @@
         <v>901436732</v>
       </c>
       <c r="G7" s="67">
-        <f>H7/$H$10*100%</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H7" s="3">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -2186,11 +2185,10 @@
         <v>939826562</v>
       </c>
       <c r="G8" s="67">
-        <f t="shared" ref="G8:G9" si="0">H8/$H$10*100%</f>
-        <v>0.18604651162790697</v>
+        <v>0.2</v>
       </c>
       <c r="H8" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -2208,20 +2206,22 @@
         <v>903371927</v>
       </c>
       <c r="G9" s="67">
-        <f t="shared" si="0"/>
-        <v>0.81395348837209303</v>
+        <v>0.6</v>
       </c>
       <c r="H9" s="3">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="55"/>
       <c r="D10" s="57"/>
-      <c r="G10" s="67"/>
+      <c r="G10" s="67">
+        <f>SUM(G7:G9)</f>
+        <v>1</v>
+      </c>
       <c r="H10" s="3">
         <f>SUM(H7:H9)</f>
-        <v>86</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -2314,9 +2314,6 @@
     <hyperlink ref="E8" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="G7:G9" calculatedColumn="1"/>
-  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId4"/>
   </tableParts>
@@ -2332,11 +2329,11 @@
   <dimension ref="A1:BQ87"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="12" ySplit="6" topLeftCell="P67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="6" topLeftCell="M11" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3149,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="K15" s="65">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3930,7 +3927,7 @@
       </c>
       <c r="F42" s="41">
         <f>SUM(F45:F51)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G42" s="64"/>
       <c r="H42" s="64"/>
@@ -3947,7 +3944,7 @@
       </c>
       <c r="F43" s="41">
         <f>SUM(F51,F45:F47)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G43" s="64"/>
       <c r="H43" s="64"/>
@@ -4184,7 +4181,9 @@
       <c r="E51" s="69" t="s">
         <v>144</v>
       </c>
-      <c r="F51" s="38"/>
+      <c r="F51" s="38">
+        <v>1</v>
+      </c>
       <c r="G51" s="64">
         <v>15</v>
       </c>
@@ -4407,7 +4406,7 @@
       <c r="E60" s="43"/>
       <c r="F60" s="43">
         <f>SUM(F8,F14,F22,F36,F42,F52)</f>
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -4503,6 +4502,9 @@
   </conditionalFormatting>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="42" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F54" formulaRange="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">

</xml_diff>